<commit_message>
edit image and questions file
</commit_message>
<xml_diff>
--- a/Knives Out/questions.xlsx
+++ b/Knives Out/questions.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanhuston/Buzzquiz/Knives Out/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CE732E5A-D6B7-D848-A6A4-BFA578B081AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF79B3B-E615-CD47-8E0B-D061CD30FBC0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="questions" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="74">
   <si>
-    <t>Which "Knives Out" character are you?</t>
-  </si>
-  <si>
     <t>How do your friends describe you?</t>
   </si>
   <si>
@@ -242,12 +239,15 @@
   </si>
   <si>
     <t>Suit.jpg</t>
+  </si>
+  <si>
+    <t>Which Knives Out character are you?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1081,11 +1081,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1100,34 +1100,34 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
         <v>5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1147,7 +1147,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -1167,7 +1167,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1187,7 +1187,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1207,7 +1207,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -1227,7 +1227,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -1247,29 +1247,29 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
         <v>5</v>
-      </c>
-      <c r="F13" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -1289,7 +1289,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1309,7 +1309,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1329,7 +1329,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -1349,7 +1349,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -1369,7 +1369,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1389,29 +1389,29 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
         <v>5</v>
-      </c>
-      <c r="F22" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -1431,7 +1431,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -1451,7 +1451,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25">
         <v>4</v>
@@ -1471,7 +1471,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26">
         <v>3</v>
@@ -1491,7 +1491,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -1531,29 +1531,29 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" t="s">
         <v>5</v>
-      </c>
-      <c r="F31" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -1573,7 +1573,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -1593,7 +1593,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -1613,7 +1613,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -1633,7 +1633,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36">
         <v>4</v>
@@ -1653,7 +1653,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -1673,29 +1673,29 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E40" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" t="s">
         <v>5</v>
-      </c>
-      <c r="F40" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -1715,7 +1715,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -1735,7 +1735,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B43">
         <v>3</v>
@@ -1755,7 +1755,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1795,29 +1795,29 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E48" t="s">
+        <v>4</v>
+      </c>
+      <c r="F48" t="s">
         <v>5</v>
-      </c>
-      <c r="F48" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B49">
         <v>2</v>
@@ -1837,7 +1837,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B50">
         <v>2</v>
@@ -1857,7 +1857,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -1877,7 +1877,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -1897,7 +1897,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B53">
         <v>2</v>
@@ -1917,7 +1917,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -1937,29 +1937,29 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E57" t="s">
+        <v>4</v>
+      </c>
+      <c r="F57" t="s">
         <v>5</v>
-      </c>
-      <c r="F57" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B58">
         <v>3</v>
@@ -1979,7 +1979,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B59">
         <v>3</v>
@@ -1999,7 +1999,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -2019,7 +2019,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -2039,7 +2039,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B62">
         <v>3</v>
@@ -2059,7 +2059,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B63">
         <v>3</v>
@@ -2079,29 +2079,29 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E66" t="s">
+        <v>4</v>
+      </c>
+      <c r="F66" t="s">
         <v>5</v>
-      </c>
-      <c r="F66" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B67">
         <v>3</v>
@@ -2121,7 +2121,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -2141,7 +2141,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -2161,7 +2161,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B70">
         <v>3</v>
@@ -2181,7 +2181,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B71">
         <v>2</v>
@@ -2201,7 +2201,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B72">
         <v>4</v>
@@ -2221,29 +2221,29 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D75" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E75" t="s">
+        <v>4</v>
+      </c>
+      <c r="F75" t="s">
         <v>5</v>
-      </c>
-      <c r="F75" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -2263,7 +2263,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B77">
         <v>4</v>
@@ -2283,7 +2283,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B78">
         <v>3</v>
@@ -2303,7 +2303,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -2323,7 +2323,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -2343,7 +2343,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -2363,29 +2363,29 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D84" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E84" t="s">
+        <v>4</v>
+      </c>
+      <c r="F84" t="s">
         <v>5</v>
-      </c>
-      <c r="F84" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B85">
         <v>4</v>
@@ -2405,7 +2405,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B86">
         <v>2</v>
@@ -2425,7 +2425,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B87">
         <v>3</v>
@@ -2445,7 +2445,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B88">
         <v>3</v>
@@ -2465,7 +2465,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B89">
         <v>2</v>

</xml_diff>